<commit_message>
Added value ETFs for ESG and Non-ESG lists
</commit_message>
<xml_diff>
--- a/extras/etfs_list.xlsx
+++ b/extras/etfs_list.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://villanova-my.sharepoint.com/personal/espinnra_villanova_edu/Documents/senior project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catal\Desktop\python\senior-project-icbm\extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BB5BDBE-E4BE-4EE0-B378-5EB6D1243B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8F749B-9691-41EF-B6E0-3C1485B06333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F8282936-D7FE-429C-8C28-2EB97C81E5CD}"/>
   </bookViews>
   <sheets>
-    <sheet name="ETFs" sheetId="2" r:id="rId1"/>
+    <sheet name="Non-ESG" sheetId="2" r:id="rId1"/>
+    <sheet name="ESG" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,17 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="112">
   <si>
     <t>Category</t>
   </si>
   <si>
-    <t>Non-ESG</t>
-  </si>
-  <si>
-    <t>ESG</t>
-  </si>
-  <si>
     <t>Large Cap</t>
   </si>
   <si>
@@ -280,13 +275,109 @@
   </si>
   <si>
     <t>Mid Cap Equity</t>
+  </si>
+  <si>
+    <t>Value ETFs</t>
+  </si>
+  <si>
+    <t>VLUE</t>
+  </si>
+  <si>
+    <t>HDV</t>
+  </si>
+  <si>
+    <t>FDL</t>
+  </si>
+  <si>
+    <t>iShares MSCI USA Value Factor ETF</t>
+  </si>
+  <si>
+    <t>iShares Core High Dividend ETF</t>
+  </si>
+  <si>
+    <t>First Trust Morningstar Dividend Leaders Index Fund</t>
+  </si>
+  <si>
+    <t>First Trust</t>
+  </si>
+  <si>
+    <t>Value &amp; Growth ETFs</t>
+  </si>
+  <si>
+    <t>VOE</t>
+  </si>
+  <si>
+    <t>Vanguard Mid-Cap Value ETF</t>
+  </si>
+  <si>
+    <t>IWS</t>
+  </si>
+  <si>
+    <t>iShares Russell Mid-Cap Value ETF</t>
+  </si>
+  <si>
+    <t>IJJ</t>
+  </si>
+  <si>
+    <t>iShares S&amp;P Mid-Cap 400 Value ETF</t>
+  </si>
+  <si>
+    <t>iShares MSCI EAFE Value ETF</t>
+  </si>
+  <si>
+    <t>EFV</t>
+  </si>
+  <si>
+    <t>Xtrackers MSCI EAFE High Dividend Yield Equity ETF</t>
+  </si>
+  <si>
+    <t>HDEF</t>
+  </si>
+  <si>
+    <t>DTH</t>
+  </si>
+  <si>
+    <t>WisdomTree International High Dividend Fund</t>
+  </si>
+  <si>
+    <t>WisdomTree</t>
+  </si>
+  <si>
+    <t>Value &amp; Growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value </t>
+  </si>
+  <si>
+    <t>NULV</t>
+  </si>
+  <si>
+    <t>Nuveen ESG Large-Cap Value ETF</t>
+  </si>
+  <si>
+    <t>TIAA</t>
+  </si>
+  <si>
+    <t>ESGN</t>
+  </si>
+  <si>
+    <t>Columbia Sustainable International Equity Income ETF</t>
+  </si>
+  <si>
+    <t>Ameriprise Financial</t>
+  </si>
+  <si>
+    <t>Non-ESG ETFs</t>
+  </si>
+  <si>
+    <t>ESG ETFs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,16 +414,50 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -437,13 +562,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFA3A3A3"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFA3A3A3"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -454,6 +590,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -463,30 +626,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -804,16 +969,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5AC97B-6637-452E-A020-67CD970CCDBA}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" customWidth="1"/>
     <col min="5" max="5" width="15.44140625" customWidth="1"/>
@@ -821,382 +986,772 @@
     <col min="7" max="7" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B2" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="17"/>
+      <c r="B3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="B4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-    </row>
-    <row r="2" spans="1:9" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13"/>
-      <c r="B2" s="2" t="s">
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="14"/>
+      <c r="B5" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="15"/>
+      <c r="B6" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14"/>
+      <c r="B8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="15"/>
+      <c r="B9" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="64.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="14"/>
+      <c r="B11" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="15"/>
+      <c r="B12" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="14"/>
+      <c r="B14" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="98.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="15"/>
+      <c r="B15" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11"/>
+      <c r="B17" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="12"/>
+      <c r="B18" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G11" r:id="rId1" display="https://etfdb.com/issuer/deutsche-bank/" xr:uid="{23BAD228-FAB1-4AD7-9276-12A41FD3A109}"/>
+    <hyperlink ref="G12" r:id="rId2" display="https://etfdb.com/issuer/wisdomtree/" xr:uid="{D498824F-83A4-4941-91F7-AD651B373DA5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC35C959-9236-484F-BAEF-01BE2471C2A9}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView zoomScale="63" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="B1" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+    </row>
+    <row r="2" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:7" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="17"/>
+      <c r="B3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="14"/>
+      <c r="B5" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="15"/>
+      <c r="B6" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14"/>
+      <c r="B8" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="15"/>
+      <c r="B9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" ht="70.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="14"/>
+      <c r="B11" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="15"/>
+      <c r="B12" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" ht="56.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="14"/>
+      <c r="B14" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="15"/>
+      <c r="B15" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
-      <c r="B8" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
-      <c r="B11" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
-      <c r="B13" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
-      <c r="B14" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="42.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" s="14" t="s">
+      <c r="B16" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11"/>
+      <c r="B17" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="12"/>
+      <c r="B18" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
-      <c r="B16" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="14" t="s">
+      <c r="E18" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F18" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
-      <c r="B17" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
+      <c r="G18" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
+  <mergeCells count="9">
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dynamically passing all tickers symbols to answers.html
</commit_message>
<xml_diff>
--- a/extras/etfs_list.xlsx
+++ b/extras/etfs_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catal\Desktop\python\senior-project-icbm\extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1301DC-67F2-4C30-A40C-41F386F6A055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D92D0D-1EC6-41BD-92BD-5E72704E9F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{F8282936-D7FE-429C-8C28-2EB97C81E5CD}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11325" xr2:uid="{F8282936-D7FE-429C-8C28-2EB97C81E5CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Non-ESG" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="143">
   <si>
     <t>Category</t>
   </si>
@@ -725,6 +725,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -761,22 +770,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1097,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5AC97B-6637-452E-A020-67CD970CCDBA}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="63" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="63" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,70 +1115,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:10" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="8" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="21" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="21"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" ht="43.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="22" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1210,7 +1210,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
@@ -1240,7 +1240,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1270,7 +1270,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="17" t="s">
         <v>79</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1302,7 +1302,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
@@ -1332,7 +1332,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
@@ -1362,7 +1362,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="17" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1394,7 +1394,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="64.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="5" t="s">
         <v>34</v>
       </c>
@@ -1424,7 +1424,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="5" t="s">
         <v>36</v>
       </c>
@@ -1454,7 +1454,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="17" t="s">
         <v>46</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1475,9 +1475,18 @@
       <c r="G13" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="H13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="5" t="s">
         <v>49</v>
       </c>
@@ -1496,9 +1505,18 @@
       <c r="G14" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="H14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="98.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="5" t="s">
         <v>51</v>
       </c>
@@ -1517,9 +1535,18 @@
       <c r="G15" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="H15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="14" t="s">
         <v>78</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1540,9 +1567,18 @@
       <c r="G16" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="67.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
+      <c r="H16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="67.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
       <c r="B17" s="5" t="s">
         <v>62</v>
       </c>
@@ -1561,9 +1597,18 @@
       <c r="G17" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+      <c r="H17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16"/>
       <c r="B18" s="5" t="s">
         <v>65</v>
       </c>
@@ -1582,8 +1627,17 @@
       <c r="G18" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
     </row>
   </sheetData>
@@ -1612,8 +1666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC35C959-9236-484F-BAEF-01BE2471C2A9}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="63" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="A10" zoomScale="63" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,69 +1685,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="21" t="s">
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="21"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="23" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="9" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1725,7 +1779,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
@@ -1749,7 +1803,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
@@ -1773,7 +1827,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="17" t="s">
         <v>79</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1805,7 +1859,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="5" t="s">
         <v>26</v>
       </c>
@@ -1829,7 +1883,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
@@ -1847,7 +1901,7 @@
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" ht="72.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="17" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1878,8 +1932,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
+    <row r="11" spans="1:10" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
       <c r="B11" s="5" t="s">
         <v>40</v>
       </c>
@@ -1903,7 +1957,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="5" t="s">
         <v>43</v>
       </c>
@@ -1921,7 +1975,7 @@
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" ht="80.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="17" t="s">
         <v>46</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1942,12 +1996,18 @@
       <c r="G13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
+      <c r="H13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18"/>
       <c r="B14" s="5" t="s">
         <v>55</v>
       </c>
@@ -1966,12 +2026,18 @@
       <c r="G14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
+      <c r="H14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
       <c r="B15" s="5" t="s">
         <v>57</v>
       </c>
@@ -1990,12 +2056,18 @@
       <c r="G15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" ht="44.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="H15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="72.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
         <v>78</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -2016,12 +2088,18 @@
       <c r="G16" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="H16" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="5" t="s">
         <v>71</v>
       </c>
@@ -2040,12 +2118,18 @@
       <c r="G17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="H17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="5" t="s">
         <v>73</v>
       </c>
@@ -2064,9 +2148,15 @@
       <c r="G18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="H18" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>

</xml_diff>